<commit_message>
updated images and principles
</commit_message>
<xml_diff>
--- a/schemes/pinouts.xlsx
+++ b/schemes/pinouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f92a95b8a3ebd29/Dokumentumok/wro2022-fe-template/schemes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csabi\Documents\GitHub\WRO2025-FE-StormsNGR\schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="8_{4D398EB6-84DA-43A4-9D8F-54E6CE081F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B780DF9-F16E-453A-AFE5-D0CDC0968B50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4446A5C8-ED12-4970-AF6D-6AA9A57BFA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BAD00418-F06A-4B00-923B-8C735A73B583}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{BAD00418-F06A-4B00-923B-8C735A73B583}"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>L&amp;K GND</t>
   </si>
@@ -72,9 +72,6 @@
     <t>LIDAR GND</t>
   </si>
   <si>
-    <t>LIDAR NC</t>
-  </si>
-  <si>
     <t>LIDAR UART TXD</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
   </si>
   <si>
     <t>Motor_DIR2</t>
-  </si>
-  <si>
-    <t>Motor_PWM2</t>
   </si>
   <si>
     <t>IMU_RXD</t>
@@ -203,6 +197,9 @@
   </si>
   <si>
     <t>PSU 5V</t>
+  </si>
+  <si>
+    <t>LiDAR PWM</t>
   </si>
 </sst>
 </file>
@@ -834,80 +831,76 @@
   <dimension ref="B1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" customWidth="1"/>
-    <col min="4" max="4" width="0.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.83203125" customWidth="1"/>
+    <col min="4" max="4" width="0.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.27734375" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="11"/>
       <c r="H3" s="5"/>
       <c r="I3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="H4" s="6"/>
       <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="H5" s="2"/>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="H6" s="4"/>
       <c r="I6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="14" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="16" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="7" t="s">
         <v>3</v>
       </c>
@@ -917,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -937,156 +930,151 @@
   </sheetPr>
   <dimension ref="A3:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="88" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="5" width="4.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" customWidth="1"/>
-    <col min="17" max="17" width="4.28515625" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="20" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="3.71875" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.71875" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" customWidth="1"/>
+    <col min="15" max="15" width="3.71875" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="17" max="17" width="4.27734375" customWidth="1"/>
+    <col min="18" max="18" width="3.71875" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" customWidth="1"/>
+    <col min="20" max="20" width="4.27734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3"/>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" s="5"/>
       <c r="K3" s="6"/>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F6" t="s">
+      <c r="O8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F8" t="s">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
       <c r="G13" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="14"/>
       <c r="K14" s="1"/>
       <c r="L14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="21" spans="3:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5"/>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G21" s="5"/>
     </row>
@@ -1105,173 +1093,171 @@
   <dimension ref="A5:S24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.71875" customWidth="1"/>
     <col min="9" max="10" width="4" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" customWidth="1"/>
+    <col min="18" max="18" width="4.44140625" customWidth="1"/>
+    <col min="19" max="19" width="13.71875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5"/>
       <c r="R6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="S6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
       </c>
       <c r="B7" s="10"/>
       <c r="R7" s="5"/>
       <c r="S7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="R10" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="S10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="R11" s="2"/>
       <c r="S11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2"/>
       <c r="R13" s="5"/>
       <c r="S13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="R15" s="5"/>
       <c r="S15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R17" s="6"/>
       <c r="S17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
       <c r="B20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I23" s="3"/>
       <c r="J23" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="151.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="151.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I24" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1287,86 +1273,86 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="9" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J23" s="5"/>
       <c r="L23" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>